<commit_message>
the raw data from airbrushing is complete
</commit_message>
<xml_diff>
--- a/Transplants_Raw_Master.xlsx
+++ b/Transplants_Raw_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayrlindsay/Desktop/GITHUB/TLPR21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2760370-5AA9-1E49-84DE-0704CF75603D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30169F84-24FF-FC44-8FE7-A38313621745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="24820" windowHeight="13840" xr2:uid="{9F99DBB5-C4DA-A948-85BF-A7F1A69C1BCE}"/>
+    <workbookView xWindow="60" yWindow="500" windowWidth="24820" windowHeight="13840" xr2:uid="{9F99DBB5-C4DA-A948-85BF-A7F1A69C1BCE}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2633" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2787" uniqueCount="204">
   <si>
     <t>Species</t>
   </si>
@@ -636,6 +636,18 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>HLE</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Some spilled when transferring homogenate</t>
   </si>
 </sst>
 </file>
@@ -1073,9 +1085,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFED04EC-AF48-A04F-A9D1-211D7C4EE961}">
   <dimension ref="A1:S282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" zoomScale="125" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q283" sqref="Q283"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K222" sqref="K222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12177,7 +12189,42 @@
       <c r="F190" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G190" s="6"/>
+      <c r="H190" s="13">
+        <v>44718</v>
+      </c>
+      <c r="I190" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="J190" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K190" s="8">
+        <v>44718</v>
+      </c>
+      <c r="L190" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M190" s="1">
+        <v>9</v>
+      </c>
+      <c r="N190" s="1">
+        <v>10</v>
+      </c>
+      <c r="O190" s="1">
+        <v>11</v>
+      </c>
+      <c r="P190" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q190" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R190" s="8">
+        <v>44354</v>
+      </c>
+      <c r="S190" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="191" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="str">
@@ -12200,6 +12247,42 @@
         <v>9</v>
       </c>
       <c r="G191" s="6"/>
+      <c r="H191" s="8">
+        <v>44698</v>
+      </c>
+      <c r="I191" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="J191" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K191" s="8">
+        <v>44698</v>
+      </c>
+      <c r="L191" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M191" s="1">
+        <v>9</v>
+      </c>
+      <c r="N191" s="1">
+        <v>10</v>
+      </c>
+      <c r="O191" s="1">
+        <v>11</v>
+      </c>
+      <c r="P191" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q191" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R191" s="8">
+        <v>44706</v>
+      </c>
+      <c r="S191" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="192" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="str">
@@ -12222,6 +12305,42 @@
         <v>9</v>
       </c>
       <c r="G192" s="6"/>
+      <c r="H192" s="8">
+        <v>44714</v>
+      </c>
+      <c r="I192" s="1">
+        <v>13</v>
+      </c>
+      <c r="J192" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K192" s="8">
+        <v>44714</v>
+      </c>
+      <c r="L192" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M192" s="1">
+        <v>9</v>
+      </c>
+      <c r="N192" s="1">
+        <v>10</v>
+      </c>
+      <c r="O192" s="1">
+        <v>11</v>
+      </c>
+      <c r="P192" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q192" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R192" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S192" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="193" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="str">
@@ -12304,6 +12423,42 @@
         <v>9</v>
       </c>
       <c r="G194" s="6"/>
+      <c r="H194" s="8">
+        <v>44714</v>
+      </c>
+      <c r="I194" s="1">
+        <v>15</v>
+      </c>
+      <c r="J194" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K194" s="8">
+        <v>44714</v>
+      </c>
+      <c r="L194" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M194" s="1">
+        <v>9</v>
+      </c>
+      <c r="N194" s="1">
+        <v>10</v>
+      </c>
+      <c r="O194" s="1">
+        <v>11</v>
+      </c>
+      <c r="P194" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q194" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R194" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S194" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="195" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="str">
@@ -12386,6 +12541,42 @@
         <v>41</v>
       </c>
       <c r="G196" s="6"/>
+      <c r="H196" s="8">
+        <v>44698</v>
+      </c>
+      <c r="I196" s="1">
+        <v>17</v>
+      </c>
+      <c r="J196" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K196" s="8">
+        <v>44698</v>
+      </c>
+      <c r="L196" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M196" s="1">
+        <v>9</v>
+      </c>
+      <c r="N196" s="1">
+        <v>10</v>
+      </c>
+      <c r="O196" s="1">
+        <v>11</v>
+      </c>
+      <c r="P196" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q196" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R196" s="8">
+        <v>44706</v>
+      </c>
+      <c r="S196" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="197" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="str">
@@ -12408,6 +12599,42 @@
         <v>42</v>
       </c>
       <c r="G197" s="6"/>
+      <c r="H197" s="8">
+        <v>44713</v>
+      </c>
+      <c r="I197" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="J197" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K197" s="8">
+        <v>44713</v>
+      </c>
+      <c r="L197" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M197" s="1">
+        <v>9</v>
+      </c>
+      <c r="N197" s="1">
+        <v>10</v>
+      </c>
+      <c r="O197" s="1">
+        <v>11</v>
+      </c>
+      <c r="P197" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q197" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R197" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S197" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="198" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="str">
@@ -12427,9 +12654,47 @@
         <v>93</v>
       </c>
       <c r="F198" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G198" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="G198" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H198" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I198" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J198" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K198" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L198" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M198" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N198" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O198" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P198" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q198" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R198" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="S198" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="199" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="str">
@@ -12452,6 +12717,42 @@
         <v>42</v>
       </c>
       <c r="G199" s="6"/>
+      <c r="H199" s="8">
+        <v>44706</v>
+      </c>
+      <c r="I199" s="1">
+        <v>19</v>
+      </c>
+      <c r="J199" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K199" s="8">
+        <v>44706</v>
+      </c>
+      <c r="L199" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M199" s="1">
+        <v>9</v>
+      </c>
+      <c r="N199" s="1">
+        <v>10</v>
+      </c>
+      <c r="O199" s="1">
+        <v>11</v>
+      </c>
+      <c r="P199" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q199" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R199" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S199" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="200" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="str">
@@ -12654,6 +12955,42 @@
         <v>41</v>
       </c>
       <c r="G203" s="6"/>
+      <c r="H203" s="8">
+        <v>44705</v>
+      </c>
+      <c r="I203" s="1">
+        <v>15</v>
+      </c>
+      <c r="J203" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K203" s="8">
+        <v>44705</v>
+      </c>
+      <c r="L203" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M203" s="1">
+        <v>9</v>
+      </c>
+      <c r="N203" s="1">
+        <v>10</v>
+      </c>
+      <c r="O203" s="1">
+        <v>11</v>
+      </c>
+      <c r="P203" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q203" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R203" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S203" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="204" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="str">
@@ -12676,6 +13013,42 @@
         <v>42</v>
       </c>
       <c r="G204" s="6"/>
+      <c r="H204" s="8">
+        <v>44714</v>
+      </c>
+      <c r="I204" s="1">
+        <v>13</v>
+      </c>
+      <c r="J204" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K204" s="8">
+        <v>44714</v>
+      </c>
+      <c r="L204" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M204" s="1">
+        <v>9</v>
+      </c>
+      <c r="N204" s="1">
+        <v>10</v>
+      </c>
+      <c r="O204" s="1">
+        <v>11</v>
+      </c>
+      <c r="P204" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q204" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R204" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S204" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="205" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="str">
@@ -12818,6 +13191,42 @@
         <v>9</v>
       </c>
       <c r="G207" s="6"/>
+      <c r="H207" s="8">
+        <v>44698</v>
+      </c>
+      <c r="I207" s="1">
+        <v>18</v>
+      </c>
+      <c r="J207" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K207" s="8">
+        <v>44698</v>
+      </c>
+      <c r="L207" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M207" s="1">
+        <v>9</v>
+      </c>
+      <c r="N207" s="1">
+        <v>10</v>
+      </c>
+      <c r="O207" s="1">
+        <v>11</v>
+      </c>
+      <c r="P207" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q207" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R207" s="8">
+        <v>44706</v>
+      </c>
+      <c r="S207" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="208" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="str">
@@ -12840,6 +13249,42 @@
         <v>41</v>
       </c>
       <c r="G208" s="6"/>
+      <c r="H208" s="8">
+        <v>44698</v>
+      </c>
+      <c r="I208" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="J208" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K208" s="8">
+        <v>44698</v>
+      </c>
+      <c r="L208" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M208" s="1">
+        <v>9</v>
+      </c>
+      <c r="N208" s="1">
+        <v>10</v>
+      </c>
+      <c r="O208" s="1">
+        <v>11</v>
+      </c>
+      <c r="P208" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q208" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R208" s="8">
+        <v>44706</v>
+      </c>
+      <c r="S208" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="209" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="str">
@@ -12862,6 +13307,42 @@
         <v>42</v>
       </c>
       <c r="G209" s="6"/>
+      <c r="H209" s="8">
+        <v>44698</v>
+      </c>
+      <c r="I209" s="1">
+        <v>18.5</v>
+      </c>
+      <c r="J209" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K209" s="8">
+        <v>44698</v>
+      </c>
+      <c r="L209" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M209" s="1">
+        <v>9</v>
+      </c>
+      <c r="N209" s="1">
+        <v>10</v>
+      </c>
+      <c r="O209" s="1">
+        <v>11</v>
+      </c>
+      <c r="P209" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q209" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R209" s="8">
+        <v>44706</v>
+      </c>
+      <c r="S209" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="210" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="str">
@@ -12944,6 +13425,42 @@
         <v>9</v>
       </c>
       <c r="G211" s="6"/>
+      <c r="H211" s="8">
+        <v>44698</v>
+      </c>
+      <c r="I211" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="J211" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K211" s="8">
+        <v>44698</v>
+      </c>
+      <c r="L211" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M211" s="1">
+        <v>9</v>
+      </c>
+      <c r="N211" s="1">
+        <v>10</v>
+      </c>
+      <c r="O211" s="1">
+        <v>11</v>
+      </c>
+      <c r="P211" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q211" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R211" s="8">
+        <v>44706</v>
+      </c>
+      <c r="S211" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="212" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="str">
@@ -12966,6 +13483,42 @@
         <v>41</v>
       </c>
       <c r="G212" s="6"/>
+      <c r="H212" s="8">
+        <v>44714</v>
+      </c>
+      <c r="I212" s="1">
+        <v>10</v>
+      </c>
+      <c r="J212" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K212" s="8">
+        <v>44714</v>
+      </c>
+      <c r="L212" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M212" s="1">
+        <v>9</v>
+      </c>
+      <c r="N212" s="1">
+        <v>10</v>
+      </c>
+      <c r="O212" s="1">
+        <v>11</v>
+      </c>
+      <c r="P212" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q212" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R212" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S212" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="213" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="str">
@@ -12988,6 +13541,42 @@
         <v>42</v>
       </c>
       <c r="G213" s="6"/>
+      <c r="H213" s="8">
+        <v>44718</v>
+      </c>
+      <c r="I213" s="1">
+        <v>13</v>
+      </c>
+      <c r="J213" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K213" s="8">
+        <v>44718</v>
+      </c>
+      <c r="L213" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M213" s="1">
+        <v>9</v>
+      </c>
+      <c r="N213" s="1">
+        <v>10</v>
+      </c>
+      <c r="O213" s="1">
+        <v>11</v>
+      </c>
+      <c r="P213" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q213" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R213" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S213" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="214" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="str">
@@ -13010,6 +13599,42 @@
         <v>41</v>
       </c>
       <c r="G214" s="6"/>
+      <c r="H214" s="8">
+        <v>44698</v>
+      </c>
+      <c r="I214" s="1">
+        <v>15</v>
+      </c>
+      <c r="J214" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K214" s="8">
+        <v>44698</v>
+      </c>
+      <c r="L214" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M214" s="1">
+        <v>9</v>
+      </c>
+      <c r="N214" s="1">
+        <v>10</v>
+      </c>
+      <c r="O214" s="1">
+        <v>11</v>
+      </c>
+      <c r="P214" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q214" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R214" s="8">
+        <v>44706</v>
+      </c>
+      <c r="S214" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="215" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="str">
@@ -13032,6 +13657,42 @@
         <v>42</v>
       </c>
       <c r="G215" s="6"/>
+      <c r="H215" s="8">
+        <v>44714</v>
+      </c>
+      <c r="I215" s="1">
+        <v>15</v>
+      </c>
+      <c r="J215" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K215" s="8">
+        <v>44714</v>
+      </c>
+      <c r="L215" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M215" s="1">
+        <v>9</v>
+      </c>
+      <c r="N215" s="1">
+        <v>10</v>
+      </c>
+      <c r="O215" s="1">
+        <v>11</v>
+      </c>
+      <c r="P215" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q215" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R215" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S215" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="216" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="str">
@@ -13054,6 +13715,42 @@
         <v>9</v>
       </c>
       <c r="G216" s="6"/>
+      <c r="H216" s="8">
+        <v>44718</v>
+      </c>
+      <c r="I216" s="1">
+        <v>12</v>
+      </c>
+      <c r="J216" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K216" s="8">
+        <v>44718</v>
+      </c>
+      <c r="L216" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M216" s="1">
+        <v>9</v>
+      </c>
+      <c r="N216" s="1">
+        <v>10</v>
+      </c>
+      <c r="O216" s="1">
+        <v>11</v>
+      </c>
+      <c r="P216" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q216" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R216" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S216" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="217" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="str">
@@ -13076,6 +13773,42 @@
         <v>41</v>
       </c>
       <c r="G217" s="6"/>
+      <c r="H217" s="8">
+        <v>44698</v>
+      </c>
+      <c r="I217" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="J217" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K217" s="8">
+        <v>44698</v>
+      </c>
+      <c r="L217" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M217" s="1">
+        <v>9</v>
+      </c>
+      <c r="N217" s="1">
+        <v>10</v>
+      </c>
+      <c r="O217" s="1">
+        <v>11</v>
+      </c>
+      <c r="P217" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q217" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R217" s="8">
+        <v>44706</v>
+      </c>
+      <c r="S217" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="218" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="str">
@@ -13098,6 +13831,42 @@
         <v>42</v>
       </c>
       <c r="G218" s="6"/>
+      <c r="H218" s="8">
+        <v>44706</v>
+      </c>
+      <c r="I218" s="1">
+        <v>12</v>
+      </c>
+      <c r="J218" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K218" s="8">
+        <v>44706</v>
+      </c>
+      <c r="L218" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M218" s="1">
+        <v>9</v>
+      </c>
+      <c r="N218" s="1">
+        <v>10</v>
+      </c>
+      <c r="O218" s="1">
+        <v>11</v>
+      </c>
+      <c r="P218" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q218" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R218" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S218" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="219" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="str">
@@ -13120,6 +13889,42 @@
         <v>9</v>
       </c>
       <c r="G219" s="6"/>
+      <c r="H219" s="8">
+        <v>44714</v>
+      </c>
+      <c r="I219" s="1">
+        <v>14</v>
+      </c>
+      <c r="J219" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K219" s="8">
+        <v>44714</v>
+      </c>
+      <c r="L219" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M219" s="1">
+        <v>9</v>
+      </c>
+      <c r="N219" s="1">
+        <v>10</v>
+      </c>
+      <c r="O219" s="1">
+        <v>11</v>
+      </c>
+      <c r="P219" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q219" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R219" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S219" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="220" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="str">
@@ -13142,6 +13947,42 @@
         <v>41</v>
       </c>
       <c r="G220" s="6"/>
+      <c r="H220" s="8">
+        <v>44698</v>
+      </c>
+      <c r="I220" s="1">
+        <v>15</v>
+      </c>
+      <c r="J220" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K220" s="8">
+        <v>44698</v>
+      </c>
+      <c r="L220" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M220" s="1">
+        <v>9</v>
+      </c>
+      <c r="N220" s="1">
+        <v>10</v>
+      </c>
+      <c r="O220" s="1">
+        <v>11</v>
+      </c>
+      <c r="P220" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q220" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R220" s="8">
+        <v>44706</v>
+      </c>
+      <c r="S220" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="221" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="str">
@@ -13164,6 +14005,42 @@
         <v>42</v>
       </c>
       <c r="G221" s="6"/>
+      <c r="H221" s="8">
+        <v>44706</v>
+      </c>
+      <c r="I221" s="1">
+        <v>20</v>
+      </c>
+      <c r="J221" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K221" s="8">
+        <v>44706</v>
+      </c>
+      <c r="L221" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M221" s="1">
+        <v>9</v>
+      </c>
+      <c r="N221" s="1">
+        <v>10</v>
+      </c>
+      <c r="O221" s="1">
+        <v>11</v>
+      </c>
+      <c r="P221" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q221" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R221" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S221" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="222" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="str">
@@ -13186,6 +14063,42 @@
         <v>40</v>
       </c>
       <c r="G222" s="6"/>
+      <c r="H222" s="8">
+        <v>44698</v>
+      </c>
+      <c r="I222" s="1">
+        <v>18</v>
+      </c>
+      <c r="J222" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K222" s="8">
+        <v>44698</v>
+      </c>
+      <c r="L222" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M222" s="1">
+        <v>9</v>
+      </c>
+      <c r="N222" s="1">
+        <v>10</v>
+      </c>
+      <c r="O222" s="1">
+        <v>11</v>
+      </c>
+      <c r="P222" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q222" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R222" s="8">
+        <v>44706</v>
+      </c>
+      <c r="S222" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="223" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="str">
@@ -13268,6 +14181,42 @@
         <v>9</v>
       </c>
       <c r="G224" s="6"/>
+      <c r="H224" s="8">
+        <v>44706</v>
+      </c>
+      <c r="I224" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="J224" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K224" s="8">
+        <v>44706</v>
+      </c>
+      <c r="L224" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M224" s="1">
+        <v>9</v>
+      </c>
+      <c r="N224" s="1">
+        <v>10</v>
+      </c>
+      <c r="O224" s="1">
+        <v>11</v>
+      </c>
+      <c r="P224" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q224" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R224" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S224" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="225" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="str">
@@ -13350,6 +14299,42 @@
         <v>9</v>
       </c>
       <c r="G226" s="6"/>
+      <c r="H226" s="8">
+        <v>44718</v>
+      </c>
+      <c r="I226" s="1">
+        <v>15</v>
+      </c>
+      <c r="J226" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K226" s="8">
+        <v>44718</v>
+      </c>
+      <c r="L226" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M226" s="1">
+        <v>9</v>
+      </c>
+      <c r="N226" s="1">
+        <v>10</v>
+      </c>
+      <c r="O226" s="1">
+        <v>11</v>
+      </c>
+      <c r="P226" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q226" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R226" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S226" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="227" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="str">
@@ -13372,6 +14357,42 @@
         <v>9</v>
       </c>
       <c r="G227" s="6"/>
+      <c r="H227" s="8">
+        <v>44706</v>
+      </c>
+      <c r="I227" s="1">
+        <v>14</v>
+      </c>
+      <c r="J227" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K227" s="8">
+        <v>44706</v>
+      </c>
+      <c r="L227" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M227" s="1">
+        <v>9</v>
+      </c>
+      <c r="N227" s="1">
+        <v>10</v>
+      </c>
+      <c r="O227" s="1">
+        <v>11</v>
+      </c>
+      <c r="P227" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q227" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R227" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S227" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="228" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="str">
@@ -13394,6 +14415,42 @@
         <v>9</v>
       </c>
       <c r="G228" s="6"/>
+      <c r="H228" s="8">
+        <v>44714</v>
+      </c>
+      <c r="I228" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="J228" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K228" s="8">
+        <v>44714</v>
+      </c>
+      <c r="L228" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M228" s="1">
+        <v>9</v>
+      </c>
+      <c r="N228" s="1">
+        <v>10</v>
+      </c>
+      <c r="O228" s="1">
+        <v>11</v>
+      </c>
+      <c r="P228" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q228" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R228" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S228" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="229" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="str">
@@ -13416,6 +14473,42 @@
         <v>9</v>
       </c>
       <c r="G229" s="6"/>
+      <c r="H229" s="8">
+        <v>44698</v>
+      </c>
+      <c r="I229" s="1">
+        <v>22.5</v>
+      </c>
+      <c r="J229" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K229" s="8">
+        <v>44698</v>
+      </c>
+      <c r="L229" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M229" s="1">
+        <v>9</v>
+      </c>
+      <c r="N229" s="1">
+        <v>10</v>
+      </c>
+      <c r="O229" s="1">
+        <v>11</v>
+      </c>
+      <c r="P229" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q229" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R229" s="8">
+        <v>44706</v>
+      </c>
+      <c r="S229" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="230" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="str">
@@ -13438,6 +14531,42 @@
         <v>9</v>
       </c>
       <c r="G230" s="6"/>
+      <c r="H230" s="8">
+        <v>44718</v>
+      </c>
+      <c r="I230" s="1">
+        <v>12</v>
+      </c>
+      <c r="J230" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K230" s="8">
+        <v>44718</v>
+      </c>
+      <c r="L230" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M230" s="1">
+        <v>9</v>
+      </c>
+      <c r="N230" s="1">
+        <v>10</v>
+      </c>
+      <c r="O230" s="1">
+        <v>11</v>
+      </c>
+      <c r="P230" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q230" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R230" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S230" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="231" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="str">
@@ -13460,6 +14589,42 @@
         <v>9</v>
       </c>
       <c r="G231" s="6"/>
+      <c r="H231" s="8">
+        <v>44713</v>
+      </c>
+      <c r="I231" s="1">
+        <v>18</v>
+      </c>
+      <c r="J231" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K231" s="8">
+        <v>44713</v>
+      </c>
+      <c r="L231" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M231" s="1">
+        <v>9</v>
+      </c>
+      <c r="N231" s="1">
+        <v>10</v>
+      </c>
+      <c r="O231" s="1">
+        <v>11</v>
+      </c>
+      <c r="P231" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q231" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R231" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S231" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="232" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="str">
@@ -13481,7 +14646,45 @@
       <c r="F232" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G232" s="6"/>
+      <c r="G232" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H232" s="8">
+        <v>44698</v>
+      </c>
+      <c r="I232" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="J232" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K232" s="8">
+        <v>44698</v>
+      </c>
+      <c r="L232" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M232" s="1">
+        <v>9</v>
+      </c>
+      <c r="N232" s="1">
+        <v>10</v>
+      </c>
+      <c r="O232" s="1">
+        <v>11</v>
+      </c>
+      <c r="P232" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q232" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R232" s="8">
+        <v>44706</v>
+      </c>
+      <c r="S232" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="233" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="str">
@@ -13504,6 +14707,42 @@
         <v>42</v>
       </c>
       <c r="G233" s="6"/>
+      <c r="H233" s="8">
+        <v>44714</v>
+      </c>
+      <c r="I233" s="1">
+        <v>11</v>
+      </c>
+      <c r="J233" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K233" s="8">
+        <v>44714</v>
+      </c>
+      <c r="L233" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M233" s="1">
+        <v>9</v>
+      </c>
+      <c r="N233" s="1">
+        <v>10</v>
+      </c>
+      <c r="O233" s="1">
+        <v>11</v>
+      </c>
+      <c r="P233" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q233" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R233" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S233" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="234" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="str">
@@ -13586,6 +14825,42 @@
         <v>41</v>
       </c>
       <c r="G235" s="6"/>
+      <c r="H235" s="8">
+        <v>44706</v>
+      </c>
+      <c r="I235" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="J235" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K235" s="8">
+        <v>44706</v>
+      </c>
+      <c r="L235" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M235" s="1">
+        <v>9</v>
+      </c>
+      <c r="N235" s="1">
+        <v>10</v>
+      </c>
+      <c r="O235" s="1">
+        <v>11</v>
+      </c>
+      <c r="P235" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q235" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R235" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S235" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="236" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="str">
@@ -13608,6 +14883,42 @@
         <v>42</v>
       </c>
       <c r="G236" s="6"/>
+      <c r="H236" s="8">
+        <v>44714</v>
+      </c>
+      <c r="I236" s="1">
+        <v>15.5</v>
+      </c>
+      <c r="J236" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K236" s="8">
+        <v>44714</v>
+      </c>
+      <c r="L236" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M236" s="1">
+        <v>9</v>
+      </c>
+      <c r="N236" s="1">
+        <v>10</v>
+      </c>
+      <c r="O236" s="1">
+        <v>11</v>
+      </c>
+      <c r="P236" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q236" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R236" s="8">
+        <v>44719</v>
+      </c>
+      <c r="S236" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="237" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="str">
@@ -14835,7 +16146,7 @@
     </row>
     <row r="258" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="str">
-        <f t="shared" ref="A258:A321" si="4">B258&amp;"_"&amp;C258&amp;"_"&amp;E258</f>
+        <f t="shared" ref="A258:A282" si="4">B258&amp;"_"&amp;C258&amp;"_"&amp;E258</f>
         <v>OFRA_PS_2GT7</v>
       </c>
       <c r="B258" s="1" t="s">
@@ -16114,7 +17425,7 @@
   <dimension ref="A2:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>